<commit_message>
remote execution in docker
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldatasheet/testdatafile.xlsx
+++ b/src/test/resources/exceldatasheet/testdatafile.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="12">
   <si>
     <t>testname</t>
   </si>
@@ -38,10 +38,19 @@
     <t>password</t>
   </si>
   <si>
+    <t>browser</t>
+  </si>
+  <si>
     <t>Admin</t>
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1206,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -1235,18 +1244,18 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="10.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1259,33 +1268,76 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>